<commit_message>
mise à jour et correction
</commit_message>
<xml_diff>
--- a/data_export/lieu_domicile.xlsx
+++ b/data_export/lieu_domicile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninamartignoni/Documents/Github/Migration-italienne/data_export/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1AB14F-E51C-E74E-97E0-29188B52D88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9523E3B-18DA-4E40-96AA-8329CB18BA12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3080" yWindow="2060" windowWidth="28040" windowHeight="17440" xr2:uid="{24350FB7-81BD-0248-8E39-B67A3FF89856}"/>
+    <workbookView xWindow="3080" yWindow="2080" windowWidth="28040" windowHeight="17440" xr2:uid="{24350FB7-81BD-0248-8E39-B67A3FF89856}"/>
   </bookViews>
   <sheets>
     <sheet name="liste_domicile" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="419">
   <si>
     <t>partie_a</t>
   </si>
@@ -635,9 +635,6 @@
     <t>Cattaneo</t>
   </si>
   <si>
-    <t>Fluer de Lys 5</t>
-  </si>
-  <si>
     <t>Cattaneo / Fluer de Lys 5</t>
   </si>
   <si>
@@ -1281,6 +1278,33 @@
   </si>
   <si>
     <t>Demoiselle Robert/ Place Neuve 2</t>
+  </si>
+  <si>
+    <t>Rue des Juifs  8</t>
+  </si>
+  <si>
+    <t>Rue de la Combe 40</t>
+  </si>
+  <si>
+    <t>Rue des Juifs 4</t>
+  </si>
+  <si>
+    <t>Rue des Juifs  2</t>
+  </si>
+  <si>
+    <t>Rue des Juifs 2</t>
+  </si>
+  <si>
+    <t>Cornes Morel 3</t>
+  </si>
+  <si>
+    <t>Rue Robert 5</t>
+  </si>
+  <si>
+    <t>Robert 6</t>
+  </si>
+  <si>
+    <t>Fleur de lys 5</t>
   </si>
 </sst>
 </file>
@@ -1303,18 +1327,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDAF2D0"/>
-        <bgColor rgb="FFDAF2D0"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1342,7 +1360,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1715,16 +1733,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B27878C5-140B-EA44-9AF2-285426ED36E1}">
   <dimension ref="A1:D342"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A319" workbookViewId="0">
-      <selection activeCell="D270" sqref="D270"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="45" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1900,7 +1918,7 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>411</v>
       </c>
       <c r="C13">
         <v>5</v>
@@ -2026,7 +2044,7 @@
         <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>410</v>
       </c>
       <c r="C22">
         <v>3</v>
@@ -2362,7 +2380,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C46">
         <v>2</v>
@@ -2404,7 +2422,7 @@
         <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>50</v>
+        <v>416</v>
       </c>
       <c r="C49">
         <v>2</v>
@@ -2446,7 +2464,7 @@
         <v>4</v>
       </c>
       <c r="B52" t="s">
-        <v>53</v>
+        <v>412</v>
       </c>
       <c r="C52">
         <v>2</v>
@@ -2558,13 +2576,13 @@
         <v>4</v>
       </c>
       <c r="B60" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C60">
         <v>2</v>
       </c>
       <c r="D60" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -2880,7 +2898,7 @@
         <v>4</v>
       </c>
       <c r="B83" t="s">
-        <v>90</v>
+        <v>415</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -3006,13 +3024,13 @@
         <v>31</v>
       </c>
       <c r="B92" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C92">
         <v>1</v>
       </c>
       <c r="D92" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
@@ -3020,7 +3038,7 @@
         <v>4</v>
       </c>
       <c r="B93" t="s">
-        <v>100</v>
+        <v>35</v>
       </c>
       <c r="C93">
         <v>1</v>
@@ -3036,8 +3054,8 @@
       <c r="B94" t="s">
         <v>101</v>
       </c>
-      <c r="C94" t="s">
-        <v>101</v>
+      <c r="C94">
+        <v>1</v>
       </c>
       <c r="D94" t="s">
         <v>101</v>
@@ -3054,7 +3072,7 @@
         <v>1</v>
       </c>
       <c r="D95" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -3062,13 +3080,13 @@
         <v>162</v>
       </c>
       <c r="B96" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C96">
         <v>1</v>
       </c>
       <c r="D96" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
@@ -3090,7 +3108,7 @@
         <v>103</v>
       </c>
       <c r="B98" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C98">
         <v>1</v>
@@ -3776,7 +3794,7 @@
         <v>162</v>
       </c>
       <c r="B147" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C147">
         <v>1</v>
@@ -3804,7 +3822,7 @@
         <v>4</v>
       </c>
       <c r="B149" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C149">
         <v>1</v>
@@ -3846,7 +3864,7 @@
         <v>4</v>
       </c>
       <c r="B152" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C152">
         <v>1</v>
@@ -3860,13 +3878,13 @@
         <v>4</v>
       </c>
       <c r="B153" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C153">
         <v>1</v>
       </c>
       <c r="D153" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
@@ -3944,7 +3962,7 @@
         <v>187</v>
       </c>
       <c r="B159" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="C159">
         <v>1</v>
@@ -4182,13 +4200,13 @@
         <v>194</v>
       </c>
       <c r="B176" t="s">
+        <v>418</v>
+      </c>
+      <c r="C176">
+        <v>1</v>
+      </c>
+      <c r="D176" t="s">
         <v>195</v>
-      </c>
-      <c r="C176">
-        <v>1</v>
-      </c>
-      <c r="D176" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
@@ -4196,27 +4214,27 @@
         <v>4</v>
       </c>
       <c r="B177" t="s">
-        <v>197</v>
+        <v>9</v>
       </c>
       <c r="C177">
         <v>1</v>
       </c>
       <c r="D177" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B178" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C178">
         <v>1</v>
       </c>
       <c r="D178" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
@@ -4224,13 +4242,13 @@
         <v>4</v>
       </c>
       <c r="B179" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C179">
         <v>1</v>
       </c>
       <c r="D179" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.2">
@@ -4238,13 +4256,13 @@
         <v>4</v>
       </c>
       <c r="B180" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C180">
         <v>1</v>
       </c>
       <c r="D180" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
@@ -4252,13 +4270,13 @@
         <v>4</v>
       </c>
       <c r="B181" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C181">
         <v>1</v>
       </c>
       <c r="D181" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
@@ -4266,27 +4284,27 @@
         <v>4</v>
       </c>
       <c r="B182" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C182">
         <v>1</v>
       </c>
       <c r="D182" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B183" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C183">
         <v>1</v>
       </c>
       <c r="D183" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
@@ -4294,13 +4312,13 @@
         <v>72</v>
       </c>
       <c r="B184" t="s">
+        <v>203</v>
+      </c>
+      <c r="C184">
+        <v>1</v>
+      </c>
+      <c r="D184" t="s">
         <v>204</v>
-      </c>
-      <c r="C184">
-        <v>1</v>
-      </c>
-      <c r="D184" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
@@ -4308,13 +4326,13 @@
         <v>4</v>
       </c>
       <c r="B185" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C185">
         <v>1</v>
       </c>
       <c r="D185" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.2">
@@ -4322,27 +4340,27 @@
         <v>4</v>
       </c>
       <c r="B186" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C186">
         <v>1</v>
       </c>
       <c r="D186" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
+        <v>207</v>
+      </c>
+      <c r="B187" t="s">
+        <v>206</v>
+      </c>
+      <c r="C187">
+        <v>1</v>
+      </c>
+      <c r="D187" t="s">
         <v>208</v>
-      </c>
-      <c r="B187" t="s">
-        <v>207</v>
-      </c>
-      <c r="C187">
-        <v>1</v>
-      </c>
-      <c r="D187" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.2">
@@ -4350,13 +4368,13 @@
         <v>4</v>
       </c>
       <c r="B188" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C188">
         <v>1</v>
       </c>
       <c r="D188" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
@@ -4364,13 +4382,13 @@
         <v>4</v>
       </c>
       <c r="B189" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C189">
         <v>1</v>
       </c>
       <c r="D189" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.2">
@@ -4378,13 +4396,13 @@
         <v>4</v>
       </c>
       <c r="B190" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C190">
         <v>1</v>
       </c>
       <c r="D190" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.2">
@@ -4392,13 +4410,13 @@
         <v>4</v>
       </c>
       <c r="B191" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C191">
         <v>1</v>
       </c>
       <c r="D191" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.2">
@@ -4406,13 +4424,13 @@
         <v>72</v>
       </c>
       <c r="B192" t="s">
+        <v>395</v>
+      </c>
+      <c r="C192">
+        <v>1</v>
+      </c>
+      <c r="D192" t="s">
         <v>396</v>
-      </c>
-      <c r="C192">
-        <v>1</v>
-      </c>
-      <c r="D192" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
@@ -4420,13 +4438,13 @@
         <v>4</v>
       </c>
       <c r="B193" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C193">
         <v>1</v>
       </c>
       <c r="D193" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
@@ -4434,27 +4452,27 @@
         <v>4</v>
       </c>
       <c r="B194" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C194">
         <v>1</v>
       </c>
       <c r="D194" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
+        <v>215</v>
+      </c>
+      <c r="B195" t="s">
         <v>216</v>
       </c>
-      <c r="B195" t="s">
+      <c r="C195">
+        <v>1</v>
+      </c>
+      <c r="D195" t="s">
         <v>217</v>
-      </c>
-      <c r="C195">
-        <v>1</v>
-      </c>
-      <c r="D195" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
@@ -4462,27 +4480,27 @@
         <v>4</v>
       </c>
       <c r="B196" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C196">
         <v>1</v>
       </c>
       <c r="D196" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
+        <v>219</v>
+      </c>
+      <c r="B197" t="s">
+        <v>218</v>
+      </c>
+      <c r="C197">
+        <v>1</v>
+      </c>
+      <c r="D197" t="s">
         <v>220</v>
-      </c>
-      <c r="B197" t="s">
-        <v>219</v>
-      </c>
-      <c r="C197">
-        <v>1</v>
-      </c>
-      <c r="D197" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
@@ -4490,13 +4508,13 @@
         <v>4</v>
       </c>
       <c r="B198" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C198">
         <v>1</v>
       </c>
       <c r="D198" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.2">
@@ -4504,13 +4522,13 @@
         <v>4</v>
       </c>
       <c r="B199" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C199">
         <v>1</v>
       </c>
       <c r="D199" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
@@ -4518,13 +4536,13 @@
         <v>4</v>
       </c>
       <c r="B200" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C200">
         <v>1</v>
       </c>
       <c r="D200" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
@@ -4532,13 +4550,13 @@
         <v>73</v>
       </c>
       <c r="B201" t="s">
+        <v>224</v>
+      </c>
+      <c r="C201">
+        <v>1</v>
+      </c>
+      <c r="D201" t="s">
         <v>225</v>
-      </c>
-      <c r="C201">
-        <v>1</v>
-      </c>
-      <c r="D201" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
@@ -4546,27 +4564,27 @@
         <v>4</v>
       </c>
       <c r="B202" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C202">
         <v>1</v>
       </c>
       <c r="D202" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B203" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C203">
         <v>1</v>
       </c>
       <c r="D203" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
@@ -4574,13 +4592,13 @@
         <v>4</v>
       </c>
       <c r="B204" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C204">
         <v>1</v>
       </c>
       <c r="D204" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
@@ -4588,41 +4606,41 @@
         <v>4</v>
       </c>
       <c r="B205" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C205">
         <v>1</v>
       </c>
       <c r="D205" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B206" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C206">
         <v>1</v>
       </c>
       <c r="D206" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B207" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C207">
         <v>1</v>
       </c>
       <c r="D207" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.2">
@@ -4630,13 +4648,13 @@
         <v>4</v>
       </c>
       <c r="B208" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C208">
         <v>1</v>
       </c>
       <c r="D208" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.2">
@@ -4644,13 +4662,13 @@
         <v>138</v>
       </c>
       <c r="B209" t="s">
+        <v>232</v>
+      </c>
+      <c r="C209">
+        <v>1</v>
+      </c>
+      <c r="D209" t="s">
         <v>233</v>
-      </c>
-      <c r="C209">
-        <v>1</v>
-      </c>
-      <c r="D209" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.2">
@@ -4658,13 +4676,13 @@
         <v>4</v>
       </c>
       <c r="B210" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C210">
         <v>1</v>
       </c>
       <c r="D210" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.2">
@@ -4672,41 +4690,41 @@
         <v>4</v>
       </c>
       <c r="B211" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C211">
         <v>1</v>
       </c>
       <c r="D211" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
+        <v>236</v>
+      </c>
+      <c r="B212" t="s">
         <v>237</v>
       </c>
-      <c r="B212" t="s">
+      <c r="C212">
+        <v>1</v>
+      </c>
+      <c r="D212" t="s">
         <v>238</v>
-      </c>
-      <c r="C212">
-        <v>1</v>
-      </c>
-      <c r="D212" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
+        <v>239</v>
+      </c>
+      <c r="B213" t="s">
         <v>240</v>
       </c>
-      <c r="B213" t="s">
+      <c r="C213">
+        <v>1</v>
+      </c>
+      <c r="D213" t="s">
         <v>241</v>
-      </c>
-      <c r="C213">
-        <v>1</v>
-      </c>
-      <c r="D213" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.2">
@@ -4714,13 +4732,13 @@
         <v>4</v>
       </c>
       <c r="B214" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C214">
         <v>1</v>
       </c>
       <c r="D214" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.2">
@@ -4728,13 +4746,13 @@
         <v>4</v>
       </c>
       <c r="B215" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C215">
         <v>1</v>
       </c>
       <c r="D215" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.2">
@@ -4742,13 +4760,13 @@
         <v>4</v>
       </c>
       <c r="B216" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C216">
         <v>1</v>
       </c>
       <c r="D216" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.2">
@@ -4756,13 +4774,13 @@
         <v>4</v>
       </c>
       <c r="B217" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C217">
         <v>1</v>
       </c>
       <c r="D217" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.2">
@@ -4770,13 +4788,13 @@
         <v>4</v>
       </c>
       <c r="B218" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C218">
         <v>1</v>
       </c>
       <c r="D218" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
@@ -4784,13 +4802,13 @@
         <v>4</v>
       </c>
       <c r="B219" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C219">
         <v>1</v>
       </c>
       <c r="D219" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">
@@ -4798,41 +4816,41 @@
         <v>4</v>
       </c>
       <c r="B220" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C220">
         <v>1</v>
       </c>
       <c r="D220" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B221" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C221">
         <v>1</v>
       </c>
       <c r="D221" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B222" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C222">
         <v>1</v>
       </c>
       <c r="D222" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.2">
@@ -4840,13 +4858,13 @@
         <v>4</v>
       </c>
       <c r="B223" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C223">
         <v>1</v>
       </c>
       <c r="D223" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
@@ -4854,27 +4872,27 @@
         <v>4</v>
       </c>
       <c r="B224" t="s">
-        <v>253</v>
+        <v>413</v>
       </c>
       <c r="C224">
         <v>1</v>
       </c>
       <c r="D224" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
+        <v>253</v>
+      </c>
+      <c r="B225" t="s">
+        <v>412</v>
+      </c>
+      <c r="C225">
+        <v>1</v>
+      </c>
+      <c r="D225" t="s">
         <v>254</v>
-      </c>
-      <c r="B225" t="s">
-        <v>53</v>
-      </c>
-      <c r="C225">
-        <v>1</v>
-      </c>
-      <c r="D225" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
@@ -4882,97 +4900,97 @@
         <v>4</v>
       </c>
       <c r="B226" t="s">
-        <v>253</v>
+        <v>414</v>
       </c>
       <c r="C226">
         <v>1</v>
       </c>
       <c r="D226" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B227" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C227">
         <v>1</v>
       </c>
       <c r="D227" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B228" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C228">
         <v>1</v>
       </c>
       <c r="D228" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B229" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C229">
         <v>1</v>
       </c>
       <c r="D229" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B230" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C230">
         <v>1</v>
       </c>
       <c r="D230" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B231" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C231">
         <v>1</v>
       </c>
       <c r="D231" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B232" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C232">
         <v>1</v>
       </c>
       <c r="D232" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.2">
@@ -4980,13 +4998,13 @@
         <v>4</v>
       </c>
       <c r="B233" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C233">
         <v>1</v>
       </c>
       <c r="D233" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.2">
@@ -4994,13 +5012,13 @@
         <v>4</v>
       </c>
       <c r="B234" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C234">
         <v>1</v>
       </c>
       <c r="D234" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.2">
@@ -5008,27 +5026,27 @@
         <v>4</v>
       </c>
       <c r="B235" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C235">
         <v>1</v>
       </c>
       <c r="D235" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
+        <v>265</v>
+      </c>
+      <c r="B236" t="s">
         <v>266</v>
       </c>
-      <c r="B236" t="s">
+      <c r="C236">
+        <v>1</v>
+      </c>
+      <c r="D236" t="s">
         <v>267</v>
-      </c>
-      <c r="C236">
-        <v>1</v>
-      </c>
-      <c r="D236" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">
@@ -5036,32 +5054,32 @@
         <v>4</v>
       </c>
       <c r="B237" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C237">
         <v>1</v>
       </c>
       <c r="D237" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
+        <v>269</v>
+      </c>
+      <c r="B238" t="s">
         <v>270</v>
       </c>
-      <c r="B238" t="s">
+      <c r="C238">
+        <v>1</v>
+      </c>
+      <c r="D238" t="s">
         <v>271</v>
-      </c>
-      <c r="C238">
-        <v>1</v>
-      </c>
-      <c r="D238" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B239" t="s">
         <v>25</v>
@@ -5070,12 +5088,12 @@
         <v>1</v>
       </c>
       <c r="D239" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B240" t="s">
         <v>25</v>
@@ -5084,7 +5102,7 @@
         <v>1</v>
       </c>
       <c r="D240" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
@@ -5092,18 +5110,18 @@
         <v>4</v>
       </c>
       <c r="B241" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C241">
         <v>1</v>
       </c>
       <c r="D241" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B242" t="s">
         <v>8</v>
@@ -5112,7 +5130,7 @@
         <v>1</v>
       </c>
       <c r="D242" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.2">
@@ -5126,7 +5144,7 @@
         <v>1</v>
       </c>
       <c r="D243" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.2">
@@ -5134,13 +5152,13 @@
         <v>4</v>
       </c>
       <c r="B244" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C244">
         <v>1</v>
       </c>
       <c r="D244" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.2">
@@ -5148,13 +5166,13 @@
         <v>4</v>
       </c>
       <c r="B245" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C245">
         <v>1</v>
       </c>
       <c r="D245" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.2">
@@ -5162,97 +5180,97 @@
         <v>4</v>
       </c>
       <c r="B246" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C246">
         <v>1</v>
       </c>
       <c r="D246" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B247" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C247">
         <v>1</v>
       </c>
       <c r="D247" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B248" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C248">
         <v>1</v>
       </c>
       <c r="D248" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B249" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C249">
         <v>1</v>
       </c>
       <c r="D249" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B250" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C250">
         <v>1</v>
       </c>
       <c r="D250" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B251" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C251">
         <v>1</v>
       </c>
       <c r="D251" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B252" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C252">
         <v>1</v>
       </c>
       <c r="D252" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.2">
@@ -5260,41 +5278,41 @@
         <v>4</v>
       </c>
       <c r="B253" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C253">
         <v>1</v>
       </c>
       <c r="D253" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B254" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C254">
         <v>1</v>
       </c>
       <c r="D254" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B255" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C255">
         <v>1</v>
       </c>
       <c r="D255" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.2">
@@ -5302,13 +5320,13 @@
         <v>4</v>
       </c>
       <c r="B256" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C256">
         <v>1</v>
       </c>
       <c r="D256" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.2">
@@ -5316,13 +5334,13 @@
         <v>4</v>
       </c>
       <c r="B257" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C257">
         <v>1</v>
       </c>
       <c r="D257" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.2">
@@ -5330,13 +5348,13 @@
         <v>4</v>
       </c>
       <c r="B258" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C258">
         <v>1</v>
       </c>
       <c r="D258" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.2">
@@ -5344,27 +5362,27 @@
         <v>4</v>
       </c>
       <c r="B259" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C259">
         <v>1</v>
       </c>
       <c r="D259" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
+        <v>293</v>
+      </c>
+      <c r="B260" t="s">
+        <v>292</v>
+      </c>
+      <c r="C260">
+        <v>1</v>
+      </c>
+      <c r="D260" t="s">
         <v>294</v>
-      </c>
-      <c r="B260" t="s">
-        <v>293</v>
-      </c>
-      <c r="C260">
-        <v>1</v>
-      </c>
-      <c r="D260" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.2">
@@ -5372,13 +5390,13 @@
         <v>4</v>
       </c>
       <c r="B261" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C261">
         <v>1</v>
       </c>
       <c r="D261" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.2">
@@ -5386,13 +5404,13 @@
         <v>4</v>
       </c>
       <c r="B262" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C262">
         <v>1</v>
       </c>
       <c r="D262" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.2">
@@ -5400,18 +5418,18 @@
         <v>4</v>
       </c>
       <c r="B263" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C263">
         <v>1</v>
       </c>
       <c r="D263" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B264" t="s">
         <v>56</v>
@@ -5420,21 +5438,21 @@
         <v>1</v>
       </c>
       <c r="D264" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
+        <v>300</v>
+      </c>
+      <c r="B265" t="s">
         <v>301</v>
       </c>
-      <c r="B265" t="s">
+      <c r="C265">
+        <v>1</v>
+      </c>
+      <c r="D265" t="s">
         <v>302</v>
-      </c>
-      <c r="C265">
-        <v>1</v>
-      </c>
-      <c r="D265" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.2">
@@ -5442,13 +5460,13 @@
         <v>4</v>
       </c>
       <c r="B266" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C266">
         <v>1</v>
       </c>
       <c r="D266" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.2">
@@ -5456,13 +5474,13 @@
         <v>4</v>
       </c>
       <c r="B267" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C267">
         <v>1</v>
       </c>
       <c r="D267" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.2">
@@ -5476,7 +5494,7 @@
         <v>1</v>
       </c>
       <c r="D268" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.2">
@@ -5484,18 +5502,18 @@
         <v>8</v>
       </c>
       <c r="B269" t="s">
+        <v>306</v>
+      </c>
+      <c r="C269">
+        <v>1</v>
+      </c>
+      <c r="D269" t="s">
         <v>307</v>
-      </c>
-      <c r="C269">
-        <v>1</v>
-      </c>
-      <c r="D269" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B270" t="s">
         <v>56</v>
@@ -5504,63 +5522,63 @@
         <v>1</v>
       </c>
       <c r="D270" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B271" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C271">
         <v>1</v>
       </c>
       <c r="D271" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B272" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C272">
         <v>1</v>
       </c>
       <c r="D272" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B273" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C273">
         <v>1</v>
       </c>
       <c r="D273" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B274" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C274">
         <v>1</v>
       </c>
       <c r="D274" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.2">
@@ -5568,13 +5586,13 @@
         <v>4</v>
       </c>
       <c r="B275" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C275">
         <v>1</v>
       </c>
       <c r="D275" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.2">
@@ -5582,13 +5600,13 @@
         <v>4</v>
       </c>
       <c r="B276" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C276">
         <v>1</v>
       </c>
       <c r="D276" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.2">
@@ -5596,13 +5614,13 @@
         <v>4</v>
       </c>
       <c r="B277" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C277">
         <v>1</v>
       </c>
       <c r="D277" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.2">
@@ -5610,13 +5628,13 @@
         <v>4</v>
       </c>
       <c r="B278" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C278">
         <v>1</v>
       </c>
       <c r="D278" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.2">
@@ -5624,13 +5642,13 @@
         <v>4</v>
       </c>
       <c r="B279" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C279">
         <v>1</v>
       </c>
       <c r="D279" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.2">
@@ -5652,13 +5670,13 @@
         <v>4</v>
       </c>
       <c r="B281" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C281">
         <v>1</v>
       </c>
       <c r="D281" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.2">
@@ -5666,13 +5684,13 @@
         <v>4</v>
       </c>
       <c r="B282" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C282">
         <v>1</v>
       </c>
       <c r="D282" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.2">
@@ -5680,32 +5698,32 @@
         <v>4</v>
       </c>
       <c r="B283" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C283">
         <v>1</v>
       </c>
       <c r="D283" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B284" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C284">
         <v>1</v>
       </c>
       <c r="D284" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B285" t="s">
         <v>31</v>
@@ -5714,21 +5732,21 @@
         <v>1</v>
       </c>
       <c r="D285" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
+        <v>324</v>
+      </c>
+      <c r="B286" t="s">
         <v>325</v>
       </c>
-      <c r="B286" t="s">
+      <c r="C286">
+        <v>1</v>
+      </c>
+      <c r="D286" t="s">
         <v>326</v>
-      </c>
-      <c r="C286">
-        <v>1</v>
-      </c>
-      <c r="D286" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.2">
@@ -5736,13 +5754,13 @@
         <v>4</v>
       </c>
       <c r="B287" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C287">
         <v>1</v>
       </c>
       <c r="D287" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.2">
@@ -5750,13 +5768,13 @@
         <v>4</v>
       </c>
       <c r="B288" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C288">
         <v>1</v>
       </c>
       <c r="D288" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.2">
@@ -5764,13 +5782,13 @@
         <v>4</v>
       </c>
       <c r="B289" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C289">
         <v>1</v>
       </c>
       <c r="D289" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.2">
@@ -5784,12 +5802,12 @@
         <v>1</v>
       </c>
       <c r="D290" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B291" t="s">
         <v>68</v>
@@ -5798,12 +5816,12 @@
         <v>1</v>
       </c>
       <c r="D291" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B292" t="s">
         <v>68</v>
@@ -5812,7 +5830,7 @@
         <v>1</v>
       </c>
       <c r="D292" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.2">
@@ -5820,13 +5838,13 @@
         <v>4</v>
       </c>
       <c r="B293" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C293">
         <v>1</v>
       </c>
       <c r="D293" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.2">
@@ -5834,18 +5852,18 @@
         <v>4</v>
       </c>
       <c r="B294" t="s">
-        <v>336</v>
+        <v>417</v>
       </c>
       <c r="C294">
         <v>1</v>
       </c>
       <c r="D294" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B295" t="s">
         <v>70</v>
@@ -5854,21 +5872,21 @@
         <v>1</v>
       </c>
       <c r="D295" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B296" t="s">
+        <v>338</v>
+      </c>
+      <c r="C296">
+        <v>1</v>
+      </c>
+      <c r="D296" t="s">
         <v>339</v>
-      </c>
-      <c r="C296">
-        <v>1</v>
-      </c>
-      <c r="D296" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.2">
@@ -5876,13 +5894,13 @@
         <v>4</v>
       </c>
       <c r="B297" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C297">
         <v>1</v>
       </c>
       <c r="D297" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.2">
@@ -5890,13 +5908,13 @@
         <v>4</v>
       </c>
       <c r="B298" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C298">
         <v>1</v>
       </c>
       <c r="D298" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.2">
@@ -5904,55 +5922,55 @@
         <v>4</v>
       </c>
       <c r="B299" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C299">
         <v>1</v>
       </c>
       <c r="D299" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B300" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C300">
         <v>1</v>
       </c>
       <c r="D300" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B301" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C301">
         <v>1</v>
       </c>
       <c r="D301" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B302" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C302">
         <v>1</v>
       </c>
       <c r="D302" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.2">
@@ -5960,13 +5978,13 @@
         <v>4</v>
       </c>
       <c r="B303" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C303">
         <v>1</v>
       </c>
       <c r="D303" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.2">
@@ -5974,13 +5992,13 @@
         <v>4</v>
       </c>
       <c r="B304" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C304">
         <v>1</v>
       </c>
       <c r="D304" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.2">
@@ -5988,13 +6006,13 @@
         <v>4</v>
       </c>
       <c r="B305" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C305">
         <v>1</v>
       </c>
       <c r="D305" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.2">
@@ -6002,13 +6020,13 @@
         <v>4</v>
       </c>
       <c r="B306" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C306">
         <v>1</v>
       </c>
       <c r="D306" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.2">
@@ -6016,27 +6034,27 @@
         <v>4</v>
       </c>
       <c r="B307" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C307">
         <v>1</v>
       </c>
       <c r="D307" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
+        <v>351</v>
+      </c>
+      <c r="B308" t="s">
         <v>352</v>
       </c>
-      <c r="B308" t="s">
+      <c r="C308">
+        <v>1</v>
+      </c>
+      <c r="D308" t="s">
         <v>353</v>
-      </c>
-      <c r="C308">
-        <v>1</v>
-      </c>
-      <c r="D308" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.2">
@@ -6044,13 +6062,13 @@
         <v>4</v>
       </c>
       <c r="B309" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C309">
         <v>1</v>
       </c>
       <c r="D309" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.2">
@@ -6058,13 +6076,13 @@
         <v>4</v>
       </c>
       <c r="B310" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C310">
         <v>1</v>
       </c>
       <c r="D310" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.2">
@@ -6072,13 +6090,13 @@
         <v>4</v>
       </c>
       <c r="B311" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C311">
         <v>1</v>
       </c>
       <c r="D311" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.2">
@@ -6086,13 +6104,13 @@
         <v>4</v>
       </c>
       <c r="B312" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C312">
         <v>1</v>
       </c>
       <c r="D312" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.2">
@@ -6125,7 +6143,7 @@
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B315" t="s">
         <v>77</v>
@@ -6134,12 +6152,12 @@
         <v>1</v>
       </c>
       <c r="D315" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B316" t="s">
         <v>77</v>
@@ -6148,35 +6166,35 @@
         <v>1</v>
       </c>
       <c r="D316" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B317" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C317">
         <v>1</v>
       </c>
       <c r="D317" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B318" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C318">
         <v>1</v>
       </c>
       <c r="D318" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.2">
@@ -6184,13 +6202,13 @@
         <v>4</v>
       </c>
       <c r="B319" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C319">
         <v>1</v>
       </c>
       <c r="D319" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.2">
@@ -6198,27 +6216,27 @@
         <v>4</v>
       </c>
       <c r="B320" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C320">
         <v>1</v>
       </c>
       <c r="D320" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
+        <v>365</v>
+      </c>
+      <c r="B321" t="s">
+        <v>368</v>
+      </c>
+      <c r="C321">
+        <v>1</v>
+      </c>
+      <c r="D321" t="s">
         <v>366</v>
-      </c>
-      <c r="B321" t="s">
-        <v>369</v>
-      </c>
-      <c r="C321">
-        <v>1</v>
-      </c>
-      <c r="D321" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.2">
@@ -6232,7 +6250,7 @@
         <v>1</v>
       </c>
       <c r="D322" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.2">
@@ -6240,18 +6258,18 @@
         <v>4</v>
       </c>
       <c r="B323" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C323">
         <v>1</v>
       </c>
       <c r="D323" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B324" t="s">
         <v>33</v>
@@ -6260,7 +6278,7 @@
         <v>1</v>
       </c>
       <c r="D324" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.2">
@@ -6268,27 +6286,27 @@
         <v>4</v>
       </c>
       <c r="B325" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C325">
         <v>1</v>
       </c>
       <c r="D325" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
+        <v>372</v>
+      </c>
+      <c r="B326" t="s">
         <v>373</v>
       </c>
-      <c r="B326" t="s">
+      <c r="C326">
+        <v>1</v>
+      </c>
+      <c r="D326" t="s">
         <v>374</v>
-      </c>
-      <c r="C326">
-        <v>1</v>
-      </c>
-      <c r="D326" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.2">
@@ -6296,13 +6314,13 @@
         <v>4</v>
       </c>
       <c r="B327" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C327">
         <v>1</v>
       </c>
       <c r="D327" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.2">
@@ -6310,55 +6328,55 @@
         <v>4</v>
       </c>
       <c r="B328" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C328">
         <v>1</v>
       </c>
       <c r="D328" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B329" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C329">
         <v>1</v>
       </c>
       <c r="D329" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B330" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C330">
         <v>1</v>
       </c>
       <c r="D330" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B331" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C331">
         <v>1</v>
       </c>
       <c r="D331" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.2">
@@ -6366,13 +6384,13 @@
         <v>4</v>
       </c>
       <c r="B332" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C332">
         <v>1</v>
       </c>
       <c r="D332" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.2">
@@ -6380,13 +6398,13 @@
         <v>4</v>
       </c>
       <c r="B333" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C333">
         <v>1</v>
       </c>
       <c r="D333" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.2">
@@ -6394,69 +6412,69 @@
         <v>4</v>
       </c>
       <c r="B334" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C334">
         <v>1</v>
       </c>
       <c r="D334" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
+        <v>383</v>
+      </c>
+      <c r="B335" t="s">
         <v>384</v>
       </c>
-      <c r="B335" t="s">
+      <c r="C335">
+        <v>1</v>
+      </c>
+      <c r="D335" t="s">
         <v>385</v>
-      </c>
-      <c r="C335">
-        <v>1</v>
-      </c>
-      <c r="D335" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B336" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C336">
         <v>1</v>
       </c>
       <c r="D336" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B337" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C337">
         <v>1</v>
       </c>
       <c r="D337" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B338" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C338">
         <v>1</v>
       </c>
       <c r="D338" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.2">
@@ -6464,13 +6482,13 @@
         <v>4</v>
       </c>
       <c r="B339" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C339">
         <v>1</v>
       </c>
       <c r="D339" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.2">
@@ -6478,13 +6496,13 @@
         <v>4</v>
       </c>
       <c r="B340" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C340">
         <v>1</v>
       </c>
       <c r="D340" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.2">
@@ -6492,13 +6510,13 @@
         <v>4</v>
       </c>
       <c r="B341" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C341">
         <v>1</v>
       </c>
       <c r="D341" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.2">
@@ -6506,13 +6524,13 @@
         <v>4</v>
       </c>
       <c r="B342" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C342">
         <v>1</v>
       </c>
       <c r="D342" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
   </sheetData>

</xml_diff>